<commit_message>
na's working, plots not
</commit_message>
<xml_diff>
--- a/df_clean.xlsx
+++ b/df_clean.xlsx
@@ -939,7 +939,7 @@
         <v>511</v>
       </c>
       <c r="M10" t="n">
-        <v>23.57</v>
+        <v>26</v>
       </c>
       <c r="N10" t="n">
         <v>-3.69</v>
@@ -1303,7 +1303,7 @@
         <v>539</v>
       </c>
       <c r="M17" t="n">
-        <v>23.57</v>
+        <v>26</v>
       </c>
       <c r="N17" t="n">
         <v>-6.14</v>
@@ -2655,7 +2655,7 @@
         <v>548</v>
       </c>
       <c r="M43" t="n">
-        <v>23.57</v>
+        <v>26</v>
       </c>
       <c r="N43" t="n">
         <v>-13.74</v>
@@ -3071,7 +3071,7 @@
         <v>548</v>
       </c>
       <c r="M51" t="n">
-        <v>23.57</v>
+        <v>26</v>
       </c>
       <c r="N51" t="n">
         <v>-14.22</v>
@@ -3591,7 +3591,7 @@
         <v>525</v>
       </c>
       <c r="M61" t="n">
-        <v>23.57</v>
+        <v>26</v>
       </c>
       <c r="N61" t="n">
         <v>-3.87</v>

</xml_diff>